<commit_message>
Nav links to maps
</commit_message>
<xml_diff>
--- a/app/data/maps.xlsx
+++ b/app/data/maps.xlsx
@@ -59,19 +59,19 @@
     <t>Zaun</t>
   </si>
   <si>
-    <t>Freljord is an unforgiving place. A mountainous land covered in snow and ice, it is home to many vicious ice storms. Travel, especially in the winter, can be very dangerous. The elements often claim even those who have spent their entire lives there. Only one storm exceeds the ones found in Freljord: the Gelid Vortex - a swirling, icy maelstrom which circles the northern hemisphere of Runeterra.</t>
-  </si>
-  <si>
     <t>Ionia is a naturally beautiful island nation full of ancient trees, tall mountains and tranquil rivers. The entire landscape is covered with large patches of forests teeming with life.</t>
   </si>
   <si>
-    <t>The human city-state of Noxus is in many ways the moral antithesis of Demacia; it is a settlement where the physically and mentally strong acquire power through any means, regardless of the consequences to their fellow citizens.</t>
-  </si>
-  <si>
-    <t>Piltover, also known as the City of Progress, is the leading center of ecologically-minded techmaturgical research on Valoran. The city's great academies and their contributions to science are known across the land, rivaled only by the eccentric colleges found in Zaun. Strangely, the coastal nation is situated atop a relatively small mountain in a vast greenish marsh. The denizens of Piltover appear to be utilizing the liquid and gases emitting from the marsh as a viable source of energy in order to power the city.</t>
-  </si>
-  <si>
-    <t>Zaun is a city-state both supported and ruined by unchecked industry, mercantilism, and magic run amok. The pollution from the countless factories and laboratories is constantly spewed into the environment. The urban heart of the city-state is often choked with smog that blocks the morning sun and drains the sky of its pastels. Visitors have called the sky the "Zaun Gray", and describe staring up at it akin to seeing the beginnings of a cosmic disturbance. As polluted as Zaun is above-ground, its subterranean levels are far worse. All of Zaun's runoff waste pools together in its sewers, mixing together into toxic and mysterious concoctions.</t>
+    <t>Freljord is an unforgiving place. A mountainous land covered in snow and ice, it is home to many vicious ice storms. Travel, especially in the winter, can be very dangerous. The elements often claim even those who have spent their entire lives there. Only one storm exceeds the ones found in Freljord: the Gelid Vortex - a swirling, icy maelstrom which circles the northern hemisphere of Runeterra.</t>
+  </si>
+  <si>
+    <t>The human city-state of Noxus is in many ways the moral antithesis of Demacia; it is a settlement where the physically and mentally strong acquire power through any means, regardless of the consequences to their fellow citizens.</t>
+  </si>
+  <si>
+    <t>Piltover, also known as the City of Progress, is the leading center of ecologically-minded techmaturgical research on Valoran. The city's great academies and their contributions to science are known across the land, rivaled only by the eccentric colleges found in Zaun. Strangely, the coastal nation is situated atop a relatively small mountain in a vast greenish marsh. The denizens of Piltover appear to be utilizing the liquid and gases emitting from the marsh as a viable source of energy in order to power the city.</t>
+  </si>
+  <si>
+    <t>Zaun is a city-state both supported and ruined by unchecked industry, mercantilism, and magic run amok. The pollution from the countless factories and laboratories is constantly spewed into the environment. The urban heart of the city-state is often choked with smog that blocks the morning sun and drains the sky of its pastels. Visitors have called the sky the "Zaun Gray", and describe staring up at it akin to seeing the beginnings of a cosmic disturbance. As polluted as Zaun is above-ground, its subterranean levels are far worse. All of Zaun's runoff waste pools together in its sewers, mixing together into toxic and mysterious concoctions.</t>
   </si>
 </sst>
 </file>
@@ -430,7 +430,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -438,7 +438,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>